<commit_message>
Add a clear button
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RequirementsAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F41F997-998D-48ED-B14E-9C6B1171B7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B6898D-EB56-4AE2-8FA7-343BACCDF7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>Data A1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,56 +78,6 @@
     <t>Data D4</t>
   </si>
   <si>
-    <t>Data a1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data a2</t>
-  </si>
-  <si>
-    <t>Data a3</t>
-  </si>
-  <si>
-    <t>Data a4</t>
-  </si>
-  <si>
-    <t>Data b1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data b2</t>
-  </si>
-  <si>
-    <t>Data c1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data c2</t>
-  </si>
-  <si>
-    <t>Data c3</t>
-  </si>
-  <si>
-    <t>Data c4</t>
-  </si>
-  <si>
-    <t>Data d1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data d2</t>
-  </si>
-  <si>
-    <t>Data d3</t>
-  </si>
-  <si>
-    <t>Data d4</t>
-  </si>
-  <si>
-    <t>Data 00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Data 01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -140,7 +90,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>貙</t>
+    <t>Datac4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -193,10 +143,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -480,18 +430,18 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
@@ -508,14 +458,14 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
@@ -560,14 +510,14 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>30</v>
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -586,69 +536,69 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1"/>
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -666,14 +616,14 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -684,5 +634,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>